<commit_message>
Projet pour des essais temporaires
</commit_message>
<xml_diff>
--- a/implementation.xlsx
+++ b/implementation.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\dev\JeuHeroMonstre\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B228A55B-55B7-4B12-B2D2-DBEE024581FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19320" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>B</t>
   </si>
@@ -48,27 +42,9 @@
     <t>typeelement</t>
   </si>
   <si>
-    <t>Personnage</t>
-  </si>
-  <si>
-    <t>Armes</t>
-  </si>
-  <si>
-    <t>Equipement</t>
-  </si>
-  <si>
-    <t>Attaquer()</t>
-  </si>
-  <si>
-    <t>Defendre()</t>
-  </si>
-  <si>
     <t>TypeEquipement</t>
   </si>
   <si>
-    <t>Parer()</t>
-  </si>
-  <si>
     <t>Monstres</t>
   </si>
   <si>
@@ -78,9 +54,6 @@
     <t>AugmenterRang()</t>
   </si>
   <si>
-    <t>Joueur</t>
-  </si>
-  <si>
     <t>Attaquer()*</t>
   </si>
   <si>
@@ -88,13 +61,46 @@
   </si>
   <si>
     <t>TypeMonstre</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Difficile</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>Personnage*(Element)</t>
+  </si>
+  <si>
+    <t>Liste&lt;Equipement&gt;</t>
+  </si>
+  <si>
+    <t>Iequipable</t>
+  </si>
+  <si>
+    <t>iarmable</t>
+  </si>
+  <si>
+    <t>Joueur*(Personnage), iarmable</t>
+  </si>
+  <si>
+    <t>Niveau</t>
+  </si>
+  <si>
+    <t>Armes: Iarmable, Iequipable</t>
+  </si>
+  <si>
+    <t>Armures: Iarmable, Iequipable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +108,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +157,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -315,6 +353,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,7 +418,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -410,7 +453,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -587,26 +630,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="10" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1">
       <c r="B1">
         <v>1</v>
       </c>
@@ -626,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>8</v>
       </c>
@@ -636,17 +681,20 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7"/>
-      <c r="I2" t="s">
+      <c r="I2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="K2" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M2" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>7</v>
       </c>
@@ -663,14 +711,17 @@
       <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="K3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>6</v>
       </c>
@@ -685,16 +736,19 @@
       <c r="F4" s="5"/>
       <c r="G4" s="3"/>
       <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>5</v>
       </c>
@@ -707,13 +761,13 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>9</v>
+      </c>
+      <c r="P5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>4</v>
       </c>
@@ -729,14 +783,11 @@
       <c r="G6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
       <c r="K6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>3</v>
       </c>
@@ -747,7 +798,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>2</v>
       </c>
@@ -762,7 +813,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:16" ht="15.75" thickBot="1">
       <c r="A9">
         <v>1</v>
       </c>
@@ -776,47 +827,66 @@
       <c r="G9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="I9" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="I10" t="s">
+      <c r="K9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="I10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="23"/>
+      <c r="M10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="I12" t="s">
         <v>12</v>
       </c>
-      <c r="M10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="M11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="M12" t="s">
+    </row>
+    <row r="14" spans="1:16">
+      <c r="K14" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="K16" s="23"/>
+    </row>
+    <row r="17" spans="9:9">
+      <c r="I17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="I13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="I14" t="s">
+    <row r="18" spans="9:9">
+      <c r="I18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9">
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9">
+      <c r="I20" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="I15" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test des interfaces et heritage
</commit_message>
<xml_diff>
--- a/implementation.xlsx
+++ b/implementation.xlsx
@@ -1,17 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\dev\JeuHeroVsMonstres\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D049CAB-C81C-4F25-B680-0047476613F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19320" windowHeight="8040"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>B</t>
   </si>
@@ -51,18 +58,12 @@
     <t>Rang</t>
   </si>
   <si>
-    <t>AugmenterRang()</t>
-  </si>
-  <si>
     <t>Attaquer()*</t>
   </si>
   <si>
     <t>Defendre()*</t>
   </si>
   <si>
-    <t>TypeMonstre</t>
-  </si>
-  <si>
     <t>Normal</t>
   </si>
   <si>
@@ -90,17 +91,44 @@
     <t>Niveau</t>
   </si>
   <si>
-    <t>Armes: Iarmable, Iequipable</t>
-  </si>
-  <si>
-    <t>Armures: Iarmable, Iequipable</t>
+    <t>AugmenterNiveau()</t>
+  </si>
+  <si>
+    <t>Equipement</t>
+  </si>
+  <si>
+    <t>Monstres*(Personnage), iarmable</t>
+  </si>
+  <si>
+    <t>typeElement</t>
+  </si>
+  <si>
+    <t>Personnage</t>
+  </si>
+  <si>
+    <t>Joueur</t>
+  </si>
+  <si>
+    <t>Armes</t>
+  </si>
+  <si>
+    <t>Armures</t>
+  </si>
+  <si>
+    <t>BonusVie</t>
+  </si>
+  <si>
+    <t>Mur</t>
+  </si>
+  <si>
+    <t>Armes*(IEquipable, iarmable)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,12 +190,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -180,7 +202,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,10 +381,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -630,28 +658,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="9" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.62890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.62890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.62890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.62890625" customWidth="1"/>
+    <col min="8" max="8" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B1">
         <v>1</v>
       </c>
@@ -662,231 +694,355 @@
         <v>3</v>
       </c>
       <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>8</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7"/>
-      <c r="I2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="E2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="J2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>7</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="I3" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="L3" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>6</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="I4" t="s">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="L4" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="P5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="L5" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" s="20" t="s">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="I10" s="24" t="s">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L12" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L13" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L14" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L15" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L16" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L18" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L19" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L20" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L21" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L22" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L23" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L24" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L25" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="23"/>
-      <c r="M10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="I11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="23"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="I12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="K14" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="K15" s="23"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="K16" s="23"/>
-    </row>
-    <row r="17" spans="9:9">
-      <c r="I17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="9:9">
-      <c r="I18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="9:9">
-      <c r="I19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="9:9">
-      <c r="I20" t="s">
-        <v>10</v>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L26" s="23" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3626DDC2-FEFE-45C5-9D77-323313A5CFD8}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6"/>
+      <c r="B2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="6"/>
+      <c r="B5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="6"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="6"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ajout des interfaces iequitable et idisposable
</commit_message>
<xml_diff>
--- a/implementation.xlsx
+++ b/implementation.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\dev\JeuHeroVsMonstres\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D049CAB-C81C-4F25-B680-0047476613F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19395" windowHeight="10395" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Classes" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Interfaces" sheetId="3" r:id="rId3"/>
+    <sheet name="Enum" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>B</t>
   </si>
@@ -121,14 +117,32 @@
     <t>Mur</t>
   </si>
   <si>
-    <t>Armes*(IEquipable, iarmable)</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Equipement*(Iequipable)</t>
+  </si>
+  <si>
+    <t>Armes*(IEquipable, iarmable, Equipementnt)</t>
+  </si>
+  <si>
+    <t>typequipement</t>
+  </si>
+  <si>
+    <t>Liste&lt;&gt;</t>
+  </si>
+  <si>
+    <t>AjouterEquipement()</t>
+  </si>
+  <si>
+    <t>EquipementActif</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -658,283 +672,215 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.62890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.62890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6.62890625" customWidth="1"/>
-    <col min="8" max="8" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="J2" s="24" t="s">
+      <c r="D2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="D5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="F5" s="22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" t="s">
         <v>9</v>
       </c>
-      <c r="J6" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="F6" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="22" t="s">
+      <c r="F7" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="24" t="s">
+      <c r="F8" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="10" spans="1:6">
+      <c r="F10" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="D11" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="D12" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="D13" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="D14" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="D15" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="D16" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6">
+      <c r="D17" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="23" t="s">
+    <row r="18" spans="4:6">
+      <c r="F18" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
+      <c r="F19" s="23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L12" s="23" t="s">
+    <row r="20" spans="4:6">
+      <c r="F20" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L13" s="22" t="s">
+    <row r="21" spans="4:6">
+      <c r="F21" s="22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L14" s="22" t="s">
+    <row r="22" spans="4:6">
+      <c r="F22" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L15" s="22" t="s">
+    <row r="23" spans="4:6">
+      <c r="F23" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L16" s="24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L18" s="21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L19" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L20" s="23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L21" s="22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L22" s="22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="12:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L23" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="12:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L24" s="23" t="s">
+    <row r="24" spans="4:6">
+      <c r="F24" s="23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="12:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L25" s="23" t="s">
+    <row r="25" spans="4:6">
+      <c r="F25" s="23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="12:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="L26" s="23" t="s">
+    <row r="26" spans="4:6">
+      <c r="F26" s="23" t="s">
         <v>21</v>
       </c>
     </row>
@@ -945,16 +891,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3626DDC2-FEFE-45C5-9D77-323313A5CFD8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6">
       <c r="A1" s="9"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -962,7 +908,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6">
       <c r="A2" s="6"/>
       <c r="B2" s="11" t="s">
         <v>3</v>
@@ -974,7 +920,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -986,7 +932,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -996,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6">
       <c r="A5" s="6"/>
       <c r="B5" s="11" t="s">
         <v>3</v>
@@ -1010,7 +956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6">
       <c r="A6" s="6"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1018,7 +964,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6">
       <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="C7" s="11" t="s">
@@ -1030,7 +976,7 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1045,4 +991,154 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>